<commit_message>
moved back to 116Cd (d,p).
</commit_message>
<xml_diff>
--- a/spectroscopic_factors/excel/116Cd_d,p_117Cd_bite_1_spec_factors.xlsx
+++ b/spectroscopic_factors/excel/116Cd_d,p_117Cd_bite_1_spec_factors.xlsx
@@ -383,7 +383,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E34"/>
+  <dimension ref="A1:E35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -414,10 +414,10 @@
         <v>0</v>
       </c>
       <c r="D2">
-        <v>0.1531158552834155</v>
+        <v>0.3883432743546536</v>
       </c>
       <c r="E2">
-        <v>0.001216015583032885</v>
+        <v>0.005801046176978834</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -428,13 +428,13 @@
         <v>107.8585558484507</v>
       </c>
       <c r="C3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D3">
-        <v>0.007578968889928035</v>
+        <v>0.009496397978399362</v>
       </c>
       <c r="E3">
-        <v>0.0002854171429053742</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -442,13 +442,13 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>134.5163962667762</v>
+        <v>107.8585558484507</v>
       </c>
       <c r="C4">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D4">
-        <v>0.4223253870688833</v>
+        <v>0.001601448494939445</v>
       </c>
       <c r="E4">
         <v>0</v>
@@ -462,10 +462,10 @@
         <v>134.5163962667762</v>
       </c>
       <c r="C5">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D5">
-        <v>0.03594088430122813</v>
+        <v>0.4223253870688833</v>
       </c>
       <c r="E5">
         <v>0</v>
@@ -476,16 +476,16 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>292.2372701306018</v>
+        <v>134.5163962667762</v>
       </c>
       <c r="C6">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="D6">
-        <v>0.01312530843239506</v>
+        <v>0.03594088430122813</v>
       </c>
       <c r="E6">
-        <v>0.0003428580233512441</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -493,16 +493,16 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>411.090801103067</v>
+        <v>292.2372701306018</v>
       </c>
       <c r="C7">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D7">
-        <v>0.00224922927944456</v>
+        <v>0.01994287695521927</v>
       </c>
       <c r="E7">
-        <v>0.0002320633383553911</v>
+        <v>0.001313111239849829</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -510,16 +510,16 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>426.2</v>
+        <v>411.090801103067</v>
       </c>
       <c r="C8">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D8">
-        <v>0.02368178790330729</v>
+        <v>0.00224922927944456</v>
       </c>
       <c r="E8">
-        <v>0.0005527690051140523</v>
+        <v>0.0002320633383553911</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -527,16 +527,16 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>442.6</v>
+        <v>426.2</v>
       </c>
       <c r="C9">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D9">
-        <v>0.04028456662544167</v>
+        <v>0.06328771551655087</v>
       </c>
       <c r="E9">
-        <v>0.0008912514740141964</v>
+        <v>0.002759137461212026</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -544,16 +544,16 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>498.0921546689657</v>
+        <v>442.6</v>
       </c>
       <c r="C10">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D10">
-        <v>0.290775837141626</v>
+        <v>0.04028456662544167</v>
       </c>
       <c r="E10">
-        <v>0.02423131976180217</v>
+        <v>0.0008912514740141964</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -561,16 +561,16 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>522.1</v>
+        <v>498.0921546689657</v>
       </c>
       <c r="C11">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D11">
-        <v>0.02843631200254661</v>
+        <v>0.1286545273913219</v>
       </c>
       <c r="E11">
-        <v>0.000734517284198621</v>
+        <v>0.003116888034738211</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -578,16 +578,16 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>627.2906398511834</v>
+        <v>522.1</v>
       </c>
       <c r="C12">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D12">
-        <v>0.01004220318482367</v>
+        <v>0.02843631200254661</v>
       </c>
       <c r="E12">
-        <v>0.0006393772121786019</v>
+        <v>0.000734517284198621</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -595,16 +595,16 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>639.4806312796794</v>
+        <v>627.2906398511834</v>
       </c>
       <c r="C13">
         <v>5</v>
       </c>
       <c r="D13">
-        <v>0.009010480277979873</v>
+        <v>0.01233653079092983</v>
       </c>
       <c r="E13">
-        <v>0.0006040203440392669</v>
+        <v>0.00110379486024109</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -612,16 +612,16 @@
         <v>12</v>
       </c>
       <c r="B14">
-        <v>665.2</v>
+        <v>639.4806312796794</v>
       </c>
       <c r="C14">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D14">
-        <v>0.06399918120629153</v>
+        <v>0.008879517077967592</v>
       </c>
       <c r="E14">
-        <v>0.001124286920312814</v>
+        <v>0.0009722098990475464</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -629,16 +629,16 @@
         <v>13</v>
       </c>
       <c r="B15">
-        <v>690.8</v>
+        <v>665.2</v>
       </c>
       <c r="C15">
         <v>2</v>
       </c>
       <c r="D15">
-        <v>0.01065132706000522</v>
+        <v>0.06399918120629153</v>
       </c>
       <c r="E15">
-        <v>0.000576664203885633</v>
+        <v>0.001124286920312814</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -646,16 +646,16 @@
         <v>14</v>
       </c>
       <c r="B16">
-        <v>699.9918964602373</v>
+        <v>690.8</v>
       </c>
       <c r="C16">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D16">
-        <v>0.001122765531301547</v>
+        <v>0.01065132706000522</v>
       </c>
       <c r="E16">
-        <v>0.0002343162847933663</v>
+        <v>0.000576664203885633</v>
       </c>
     </row>
     <row r="17" spans="1:5">
@@ -663,16 +663,16 @@
         <v>15</v>
       </c>
       <c r="B17">
-        <v>728.2049555816418</v>
+        <v>699.9918964602373</v>
       </c>
       <c r="C17">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D17">
-        <v>0.0007583871226285256</v>
+        <v>0.003474240466262073</v>
       </c>
       <c r="E17">
-        <v>0.0001516774245257051</v>
+        <v>0.001789760240195614</v>
       </c>
     </row>
     <row r="18" spans="1:5">
@@ -680,16 +680,16 @@
         <v>16</v>
       </c>
       <c r="B18">
-        <v>779.0788707099858</v>
+        <v>728.2049555816418</v>
       </c>
       <c r="C18">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D18">
-        <v>0.008661036420250534</v>
+        <v>0.0007583871226285256</v>
       </c>
       <c r="E18">
-        <v>0.0003114080510651878</v>
+        <v>0.0001516774245257051</v>
       </c>
     </row>
     <row r="19" spans="1:5">
@@ -697,16 +697,16 @@
         <v>17</v>
       </c>
       <c r="B19">
-        <v>820.1</v>
+        <v>779.0788707099858</v>
       </c>
       <c r="C19">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D19">
-        <v>0.01292736193670261</v>
+        <v>0.01325238894025671</v>
       </c>
       <c r="E19">
-        <v>0.0004812496741519585</v>
+        <v>0.001356543749790057</v>
       </c>
     </row>
     <row r="20" spans="1:5">
@@ -714,16 +714,16 @@
         <v>18</v>
       </c>
       <c r="B20">
-        <v>862.5559205640915</v>
+        <v>820.1</v>
       </c>
       <c r="C20">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D20">
-        <v>0.005992979694741703</v>
+        <v>0.01292736193670261</v>
       </c>
       <c r="E20">
-        <v>0.0004565654621896326</v>
+        <v>0.0004812496741519585</v>
       </c>
     </row>
     <row r="21" spans="1:5">
@@ -731,16 +731,16 @@
         <v>19</v>
       </c>
       <c r="B21">
-        <v>997.3547572460591</v>
+        <v>864.8217727435604</v>
       </c>
       <c r="C21">
         <v>5</v>
       </c>
       <c r="D21">
-        <v>0.005682174596704262</v>
+        <v>0.006112995676851511</v>
       </c>
       <c r="E21">
-        <v>0.0005166145765674989</v>
+        <v>0.0007485300828797769</v>
       </c>
     </row>
     <row r="22" spans="1:5">
@@ -748,16 +748,16 @@
         <v>20</v>
       </c>
       <c r="B22">
-        <v>1011.995701247272</v>
+        <v>997.3547572460591</v>
       </c>
       <c r="C22">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D22">
-        <v>0.001236450633981828</v>
+        <v>0.005240126451864466</v>
       </c>
       <c r="E22">
-        <v>0.0006545915121080266</v>
+        <v>0.0007921121380725358</v>
       </c>
     </row>
     <row r="23" spans="1:5">
@@ -765,16 +765,16 @@
         <v>21</v>
       </c>
       <c r="B23">
-        <v>1073.2</v>
+        <v>1011.995701247272</v>
       </c>
       <c r="C23">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D23">
-        <v>0.002132357724157726</v>
+        <v>0.001929248399486033</v>
       </c>
       <c r="E23">
-        <v>0.0002623138470194028</v>
+        <v>0.0004823120998715085</v>
       </c>
     </row>
     <row r="24" spans="1:5">
@@ -782,16 +782,16 @@
         <v>22</v>
       </c>
       <c r="B24">
-        <v>1082.466210769789</v>
+        <v>1073.2</v>
       </c>
       <c r="C24">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D24">
-        <v>0.02882081720112604</v>
+        <v>0.01135728761882676</v>
       </c>
       <c r="E24">
-        <v>0.001841133285575619</v>
+        <v>0.001323179140057487</v>
       </c>
     </row>
     <row r="25" spans="1:5">
@@ -799,16 +799,16 @@
         <v>23</v>
       </c>
       <c r="B25">
-        <v>1105.246920920629</v>
+        <v>1082.466210769789</v>
       </c>
       <c r="C25">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D25">
-        <v>0.005243685527966736</v>
+        <v>0.02441890964009653</v>
       </c>
       <c r="E25">
-        <v>0.0003343261806634169</v>
+        <v>0.001559930345558992</v>
       </c>
     </row>
     <row r="26" spans="1:5">
@@ -816,16 +816,16 @@
         <v>24</v>
       </c>
       <c r="B26">
-        <v>1132.989830446533</v>
+        <v>1105.246920920629</v>
       </c>
       <c r="C26">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D26">
-        <v>0.009036639692705812</v>
+        <v>0.005243685527966736</v>
       </c>
       <c r="E26">
-        <v>0.0009731765822913952</v>
+        <v>0.0003343261806634169</v>
       </c>
     </row>
     <row r="27" spans="1:5">
@@ -833,16 +833,16 @@
         <v>25</v>
       </c>
       <c r="B27">
-        <v>1221.150820773939</v>
+        <v>1132.989830446533</v>
       </c>
       <c r="C27">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D27">
-        <v>0.007077348597404069</v>
+        <v>0.009050998742610073</v>
       </c>
       <c r="E27">
-        <v>0.0002773555531415109</v>
+        <v>0.0009120918663770896</v>
       </c>
     </row>
     <row r="28" spans="1:5">
@@ -850,16 +850,16 @@
         <v>26</v>
       </c>
       <c r="B28">
-        <v>1257.056227090943</v>
+        <v>1221.150820773939</v>
       </c>
       <c r="C28">
         <v>0</v>
       </c>
       <c r="D28">
-        <v>0.005110493547277692</v>
+        <v>0.02144127001002603</v>
       </c>
       <c r="E28">
-        <v>0.0002388081096858734</v>
+        <v>0.00175241149120405</v>
       </c>
     </row>
     <row r="29" spans="1:5">
@@ -867,16 +867,16 @@
         <v>27</v>
       </c>
       <c r="B29">
-        <v>1278.325416780053</v>
+        <v>1257.056227090943</v>
       </c>
       <c r="C29">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D29">
-        <v>0.01383871555435027</v>
+        <v>0.01604363934744349</v>
       </c>
       <c r="E29">
-        <v>0.0004898660373221334</v>
+        <v>0.001542657629561874</v>
       </c>
     </row>
     <row r="30" spans="1:5">
@@ -884,16 +884,16 @@
         <v>28</v>
       </c>
       <c r="B30">
-        <v>1315.93448102085</v>
+        <v>1278.325416780053</v>
       </c>
       <c r="C30">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D30">
-        <v>0.005088656274641255</v>
+        <v>0.01383871555435027</v>
       </c>
       <c r="E30">
-        <v>0.0003673024382625725</v>
+        <v>0.0004898660373221334</v>
       </c>
     </row>
     <row r="31" spans="1:5">
@@ -901,16 +901,16 @@
         <v>29</v>
       </c>
       <c r="B31">
-        <v>1342.277962181449</v>
+        <v>1315.93448102085</v>
       </c>
       <c r="C31">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D31">
-        <v>0.003600336193038126</v>
+        <v>0.00674385453734916</v>
       </c>
       <c r="E31">
-        <v>0.0003176767229151288</v>
+        <v>0.0011055499241556</v>
       </c>
     </row>
     <row r="32" spans="1:5">
@@ -918,16 +918,16 @@
         <v>30</v>
       </c>
       <c r="B32">
-        <v>1355.9</v>
+        <v>1342.277962181449</v>
       </c>
       <c r="C32">
         <v>2</v>
       </c>
       <c r="D32">
-        <v>0.01311240045682935</v>
+        <v>0.003600336193038126</v>
       </c>
       <c r="E32">
-        <v>0.0004979392578542791</v>
+        <v>0.0003176767229151288</v>
       </c>
     </row>
     <row r="33" spans="1:5">
@@ -935,16 +935,16 @@
         <v>31</v>
       </c>
       <c r="B33">
-        <v>1475.089127951248</v>
+        <v>1355.9</v>
       </c>
       <c r="C33">
         <v>2</v>
       </c>
       <c r="D33">
-        <v>0.01791810606136577</v>
+        <v>0.01311240045682935</v>
       </c>
       <c r="E33">
-        <v>0.0006499560319044467</v>
+        <v>0.0004979392578542791</v>
       </c>
     </row>
     <row r="34" spans="1:5">
@@ -952,16 +952,33 @@
         <v>32</v>
       </c>
       <c r="B34">
+        <v>1475.089127951248</v>
+      </c>
+      <c r="C34">
+        <v>2</v>
+      </c>
+      <c r="D34">
+        <v>0.01791810606136577</v>
+      </c>
+      <c r="E34">
+        <v>0.0006499560319044467</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5">
+      <c r="A35" s="1">
+        <v>33</v>
+      </c>
+      <c r="B35">
         <v>1485.514423856088</v>
       </c>
-      <c r="C34">
+      <c r="C35">
         <v>5</v>
       </c>
-      <c r="D34">
-        <v>0.02487243180624383</v>
-      </c>
-      <c r="E34">
-        <v>0.002419862356478336</v>
+      <c r="D35">
+        <v>0.03083767517834564</v>
+      </c>
+      <c r="E35">
+        <v>0.003172829395605959</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
redid ptolemy for 116Cd(d,p) investigated bic
</commit_message>
<xml_diff>
--- a/spectroscopic_factors/excel/116Cd_d,p_117Cd_bite_1_spec_factors.xlsx
+++ b/spectroscopic_factors/excel/116Cd_d,p_117Cd_bite_1_spec_factors.xlsx
@@ -383,7 +383,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E35"/>
+  <dimension ref="A1:E34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -414,10 +414,10 @@
         <v>0</v>
       </c>
       <c r="D2">
-        <v>0.3883432743546536</v>
+        <v>0.7122645628334362</v>
       </c>
       <c r="E2">
-        <v>0.005801046176978834</v>
+        <v>0.01063976098488827</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -425,13 +425,13 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>107.8585558484507</v>
+        <v>134.5163962667762</v>
       </c>
       <c r="C3">
         <v>2</v>
       </c>
       <c r="D3">
-        <v>0.009496397978399362</v>
+        <v>0.4987642214596824</v>
       </c>
       <c r="E3">
         <v>0</v>
@@ -442,13 +442,13 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>107.8585558484507</v>
+        <v>134.5163962667762</v>
       </c>
       <c r="C4">
         <v>5</v>
       </c>
       <c r="D4">
-        <v>0.001601448494939445</v>
+        <v>0.03398050020896767</v>
       </c>
       <c r="E4">
         <v>0</v>
@@ -459,16 +459,16 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>134.5163962667762</v>
+        <v>292.2372701306018</v>
       </c>
       <c r="C5">
         <v>2</v>
       </c>
       <c r="D5">
-        <v>0.4223253870688833</v>
+        <v>0.001921716223893481</v>
       </c>
       <c r="E5">
-        <v>0</v>
+        <v>0.0001865743906692699</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -476,16 +476,16 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>134.5163962667762</v>
+        <v>338.2871738311746</v>
       </c>
       <c r="C6">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D6">
-        <v>0.03594088430122813</v>
+        <v>0.0005914237785581779</v>
       </c>
       <c r="E6">
-        <v>0</v>
+        <v>0.0001108919584796584</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -493,16 +493,16 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>292.2372701306018</v>
+        <v>411.0908011030671</v>
       </c>
       <c r="C7">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D7">
-        <v>0.01994287695521927</v>
+        <v>0.002302371894805456</v>
       </c>
       <c r="E7">
-        <v>0.001313111239849829</v>
+        <v>0.0002375463066069121</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -510,16 +510,16 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>411.090801103067</v>
+        <v>426.2</v>
       </c>
       <c r="C8">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D8">
-        <v>0.00224922927944456</v>
+        <v>0.1029265847196399</v>
       </c>
       <c r="E8">
-        <v>0.0002320633383553911</v>
+        <v>0.00448726254908512</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -527,16 +527,16 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>426.2</v>
+        <v>442.6</v>
       </c>
       <c r="C9">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D9">
-        <v>0.06328771551655087</v>
+        <v>0.04107328262549061</v>
       </c>
       <c r="E9">
-        <v>0.002759137461212026</v>
+        <v>0.0009087009430418279</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -544,16 +544,16 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>442.6</v>
+        <v>498.0921546689657</v>
       </c>
       <c r="C10">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D10">
-        <v>0.04028456662544167</v>
+        <v>0.02329854005834736</v>
       </c>
       <c r="E10">
-        <v>0.0008912514740141964</v>
+        <v>0.00194154500486228</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -561,16 +561,16 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>498.0921546689657</v>
+        <v>522.1</v>
       </c>
       <c r="C11">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D11">
-        <v>0.1286545273913219</v>
+        <v>0.02914010700358869</v>
       </c>
       <c r="E11">
-        <v>0.003116888034738211</v>
+        <v>0.0007526964908676043</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -578,16 +578,16 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>522.1</v>
+        <v>627.2906398511834</v>
       </c>
       <c r="C12">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D12">
-        <v>0.02843631200254661</v>
+        <v>0.01266002641348959</v>
       </c>
       <c r="E12">
-        <v>0.000734517284198621</v>
+        <v>0.00113273920541749</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -595,16 +595,16 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>627.2906398511834</v>
+        <v>639.4806312796794</v>
       </c>
       <c r="C13">
         <v>5</v>
       </c>
       <c r="D13">
-        <v>0.01233653079092983</v>
+        <v>0.009109340139086099</v>
       </c>
       <c r="E13">
-        <v>0.00110379486024109</v>
+        <v>0.000997373007929135</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -612,16 +612,16 @@
         <v>12</v>
       </c>
       <c r="B14">
-        <v>639.4806312796794</v>
+        <v>665.2</v>
       </c>
       <c r="C14">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D14">
-        <v>0.008879517077967592</v>
+        <v>0.06564432074864086</v>
       </c>
       <c r="E14">
-        <v>0.0009722098990475464</v>
+        <v>0.001153187428642613</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -629,16 +629,16 @@
         <v>13</v>
       </c>
       <c r="B15">
-        <v>665.2</v>
+        <v>690.8</v>
       </c>
       <c r="C15">
         <v>2</v>
       </c>
       <c r="D15">
-        <v>0.06399918120629153</v>
+        <v>0.01092269360327826</v>
       </c>
       <c r="E15">
-        <v>0.001124286920312814</v>
+        <v>0.0005913560231074218</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -646,16 +646,16 @@
         <v>14</v>
       </c>
       <c r="B16">
-        <v>690.8</v>
+        <v>699.9918964602372</v>
       </c>
       <c r="C16">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D16">
-        <v>0.01065132706000522</v>
+        <v>0.002512792308611072</v>
       </c>
       <c r="E16">
-        <v>0.000576664203885633</v>
+        <v>0.000384902480718782</v>
       </c>
     </row>
     <row r="17" spans="1:5">
@@ -663,16 +663,16 @@
         <v>15</v>
       </c>
       <c r="B17">
-        <v>699.9918964602373</v>
+        <v>728.2049555816417</v>
       </c>
       <c r="C17">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D17">
-        <v>0.003474240466262073</v>
+        <v>0.0007773338542252403</v>
       </c>
       <c r="E17">
-        <v>0.001789760240195614</v>
+        <v>0.000155466770845048</v>
       </c>
     </row>
     <row r="18" spans="1:5">
@@ -680,16 +680,16 @@
         <v>16</v>
       </c>
       <c r="B18">
-        <v>728.2049555816418</v>
+        <v>779.0788707099858</v>
       </c>
       <c r="C18">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D18">
-        <v>0.0007583871226285256</v>
+        <v>0.04320687781100344</v>
       </c>
       <c r="E18">
-        <v>0.0001516774245257051</v>
+        <v>0.003304055362017911</v>
       </c>
     </row>
     <row r="19" spans="1:5">
@@ -697,16 +697,16 @@
         <v>17</v>
       </c>
       <c r="B19">
-        <v>779.0788707099858</v>
+        <v>820.1</v>
       </c>
       <c r="C19">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D19">
-        <v>0.01325238894025671</v>
+        <v>0.01323879839570528</v>
       </c>
       <c r="E19">
-        <v>0.001356543749790057</v>
+        <v>0.0004928435859761914</v>
       </c>
     </row>
     <row r="20" spans="1:5">
@@ -714,16 +714,16 @@
         <v>18</v>
       </c>
       <c r="B20">
-        <v>820.1</v>
+        <v>864.8217727435604</v>
       </c>
       <c r="C20">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D20">
-        <v>0.01292736193670261</v>
+        <v>0.003647852649776206</v>
       </c>
       <c r="E20">
-        <v>0.0004812496741519585</v>
+        <v>0.0004234114682775954</v>
       </c>
     </row>
     <row r="21" spans="1:5">
@@ -731,16 +731,16 @@
         <v>19</v>
       </c>
       <c r="B21">
-        <v>864.8217727435604</v>
+        <v>997.354757246059</v>
       </c>
       <c r="C21">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D21">
-        <v>0.006112995676851511</v>
+        <v>0.004268312320930733</v>
       </c>
       <c r="E21">
-        <v>0.0007485300828797769</v>
+        <v>0.0005058740528510498</v>
       </c>
     </row>
     <row r="22" spans="1:5">
@@ -748,16 +748,16 @@
         <v>20</v>
       </c>
       <c r="B22">
-        <v>997.3547572460591</v>
+        <v>1011.995701247272</v>
       </c>
       <c r="C22">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D22">
-        <v>0.005240126451864466</v>
+        <v>0.004783082758831489</v>
       </c>
       <c r="E22">
-        <v>0.0007921121380725358</v>
+        <v>0.001195770689707872</v>
       </c>
     </row>
     <row r="23" spans="1:5">
@@ -765,16 +765,16 @@
         <v>21</v>
       </c>
       <c r="B23">
-        <v>1011.995701247272</v>
+        <v>1073.2</v>
       </c>
       <c r="C23">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D23">
-        <v>0.001929248399486033</v>
+        <v>0.007268349535822038</v>
       </c>
       <c r="E23">
-        <v>0.0004823120998715085</v>
+        <v>0.0005375846583847022</v>
       </c>
     </row>
     <row r="24" spans="1:5">
@@ -782,16 +782,16 @@
         <v>22</v>
       </c>
       <c r="B24">
-        <v>1073.2</v>
+        <v>1082.466210769789</v>
       </c>
       <c r="C24">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="D24">
-        <v>0.01135728761882676</v>
+        <v>0.02505997561845997</v>
       </c>
       <c r="E24">
-        <v>0.001323179140057487</v>
+        <v>0.001600882963341423</v>
       </c>
     </row>
     <row r="25" spans="1:5">
@@ -799,16 +799,16 @@
         <v>23</v>
       </c>
       <c r="B25">
-        <v>1082.466210769789</v>
+        <v>1105.246920920629</v>
       </c>
       <c r="C25">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D25">
-        <v>0.02441890964009653</v>
+        <v>0.005533321627902068</v>
       </c>
       <c r="E25">
-        <v>0.001559930345558992</v>
+        <v>0.0003529978393098491</v>
       </c>
     </row>
     <row r="26" spans="1:5">
@@ -816,16 +816,16 @@
         <v>24</v>
       </c>
       <c r="B26">
-        <v>1105.246920920629</v>
+        <v>1132.989830446533</v>
       </c>
       <c r="C26">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D26">
-        <v>0.005243685527966736</v>
+        <v>0.00930587291695033</v>
       </c>
       <c r="E26">
-        <v>0.0003343261806634169</v>
+        <v>0.0009377823177255106</v>
       </c>
     </row>
     <row r="27" spans="1:5">
@@ -833,16 +833,16 @@
         <v>25</v>
       </c>
       <c r="B27">
-        <v>1132.989830446533</v>
+        <v>1221.150820773939</v>
       </c>
       <c r="C27">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D27">
-        <v>0.009050998742610073</v>
+        <v>0.02675053742603294</v>
       </c>
       <c r="E27">
-        <v>0.0009120918663770896</v>
+        <v>0.002186342001166153</v>
       </c>
     </row>
     <row r="28" spans="1:5">
@@ -850,16 +850,16 @@
         <v>26</v>
       </c>
       <c r="B28">
-        <v>1221.150820773939</v>
+        <v>1257.056227090943</v>
       </c>
       <c r="C28">
         <v>0</v>
       </c>
       <c r="D28">
-        <v>0.02144127001002603</v>
+        <v>0.019774236949361</v>
       </c>
       <c r="E28">
-        <v>0.00175241149120405</v>
+        <v>0.001901368937438558</v>
       </c>
     </row>
     <row r="29" spans="1:5">
@@ -867,16 +867,16 @@
         <v>27</v>
       </c>
       <c r="B29">
-        <v>1257.056227090943</v>
+        <v>1278.325416780053</v>
       </c>
       <c r="C29">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D29">
-        <v>0.01604363934744349</v>
+        <v>0.01413525571574973</v>
       </c>
       <c r="E29">
-        <v>0.001542657629561874</v>
+        <v>0.0005003630341858311</v>
       </c>
     </row>
     <row r="30" spans="1:5">
@@ -884,16 +884,16 @@
         <v>28</v>
       </c>
       <c r="B30">
-        <v>1278.325416780053</v>
+        <v>1315.93448102085</v>
       </c>
       <c r="C30">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D30">
-        <v>0.01383871555435027</v>
+        <v>0.007705508831167587</v>
       </c>
       <c r="E30">
-        <v>0.0004898660373221334</v>
+        <v>0.001263198169043867</v>
       </c>
     </row>
     <row r="31" spans="1:5">
@@ -901,16 +901,16 @@
         <v>29</v>
       </c>
       <c r="B31">
-        <v>1315.93448102085</v>
+        <v>1342.277962181449</v>
       </c>
       <c r="C31">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D31">
-        <v>0.00674385453734916</v>
+        <v>0.003679677657209016</v>
       </c>
       <c r="E31">
-        <v>0.0011055499241556</v>
+        <v>0.000324677440341972</v>
       </c>
     </row>
     <row r="32" spans="1:5">
@@ -918,16 +918,16 @@
         <v>30</v>
       </c>
       <c r="B32">
-        <v>1342.277962181449</v>
+        <v>1355.9</v>
       </c>
       <c r="C32">
         <v>2</v>
       </c>
       <c r="D32">
-        <v>0.003600336193038126</v>
+        <v>0.01340149393926604</v>
       </c>
       <c r="E32">
-        <v>0.0003176767229151288</v>
+        <v>0.0005089174913645331</v>
       </c>
     </row>
     <row r="33" spans="1:5">
@@ -935,16 +935,16 @@
         <v>31</v>
       </c>
       <c r="B33">
-        <v>1355.9</v>
+        <v>1475.089127951248</v>
       </c>
       <c r="C33">
         <v>2</v>
       </c>
       <c r="D33">
-        <v>0.01311240045682935</v>
+        <v>0.01830332173056794</v>
       </c>
       <c r="E33">
-        <v>0.0004979392578542791</v>
+        <v>0.0006639292301277737</v>
       </c>
     </row>
     <row r="34" spans="1:5">
@@ -952,33 +952,16 @@
         <v>32</v>
       </c>
       <c r="B34">
-        <v>1475.089127951248</v>
+        <v>1485.514423856088</v>
       </c>
       <c r="C34">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D34">
-        <v>0.01791810606136577</v>
+        <v>0.03166765477755253</v>
       </c>
       <c r="E34">
-        <v>0.0006499560319044467</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5">
-      <c r="A35" s="1">
-        <v>33</v>
-      </c>
-      <c r="B35">
-        <v>1485.514423856088</v>
-      </c>
-      <c r="C35">
-        <v>5</v>
-      </c>
-      <c r="D35">
-        <v>0.03083767517834564</v>
-      </c>
-      <c r="E35">
-        <v>0.003172829395605959</v>
+        <v>0.003258224408520749</v>
       </c>
     </row>
   </sheetData>

</xml_diff>